<commit_message>
Added the rest of the work besides the tooltip, sidebar nav, and only one javascript widget. Drink specials table is not responsive and I cannot understand why. I'll figure out these problems in the future.
</commit_message>
<xml_diff>
--- a/docs/Assignment_2_ Rubric_S16.xlsx
+++ b/docs/Assignment_2_ Rubric_S16.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="14960" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25260" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Possible points</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>1. Create a Bootstrap sortable table</t>
+  </si>
+  <si>
+    <t>Colleen Bowes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couldn’t add the tooltip, could not find another javascript to add into the site, My drink specials sections is not responsive (Ive tried many times) and I could not figure out how to put a sidebar on when the screen went to mobile size. Ive tried many different ways but it could be my bootstrap css. </t>
   </si>
 </sst>
 </file>
@@ -859,7 +865,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:H31"/>
+      <selection activeCell="F6" sqref="F6:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -906,7 +912,9 @@
       <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -969,7 +977,7 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
@@ -1054,7 +1062,7 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
@@ -1088,7 +1096,7 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
@@ -1122,7 +1130,7 @@
         <v>10</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
@@ -1175,7 +1183,7 @@
       </c>
       <c r="E19" s="14">
         <f>SUM(E6:E18)</f>
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
@@ -1232,7 +1240,7 @@
       </c>
       <c r="E23" s="14">
         <f>SUM(E19, E21:E22)</f>
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1255,7 +1263,9 @@
     <row r="25" spans="1:9">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="22"/>
+      <c r="C25" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>

</xml_diff>